<commit_message>
Update scenario file with 2021 CO2 emissions cap on sector
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3A4C4-5EB5-4E0C-88FC-C9BAA49A9B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AABE76-4D79-4105-9F51-1D50FE30E688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26844" yWindow="3204" windowWidth="14400" windowHeight="7356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="19" r:id="rId1"/>
@@ -2177,7 +2177,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF08F70-6061-4334-B6F9-12A767772C59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CE3B6C-F45A-4A9A-83A7-260FE2022E45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2270,7 +2270,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6629FB-C09F-4200-B78E-4FD5614996BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2320,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA8B95B-A935-4706-BBFB-6D5C157F61C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2370,7 +2370,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DB6255-16F1-4131-B80B-898A983DA66E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2419,7 +2419,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C8A817-8A7F-451D-A8EF-15CA92E73ED5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -2481,7 +2481,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1104FA2-617F-40B5-9110-C12C45401468}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2536,7 +2536,7 @@
         <xdr:cNvPr id="2" name="Arrow: Right 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2972,21 +2972,21 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="50" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="50" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="50" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="50" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="50" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="50" customWidth="1"/>
+    <col min="1" max="4" width="21.7265625" style="50" customWidth="1"/>
+    <col min="5" max="6" width="14.1796875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" style="50" customWidth="1"/>
+    <col min="8" max="10" width="8.1796875" style="50" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="50" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" style="50" customWidth="1"/>
     <col min="13" max="13" width="10" style="50" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="50" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="50" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="50"/>
+    <col min="14" max="14" width="11.453125" style="50" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" style="50" customWidth="1"/>
+    <col min="16" max="16384" width="8.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="70"/>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
@@ -3014,7 +3014,7 @@
       <c r="Y1" s="71"/>
       <c r="Z1" s="71"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="70"/>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -3042,7 +3042,7 @@
       <c r="Y2" s="71"/>
       <c r="Z2" s="71"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="70"/>
       <c r="B3" s="70"/>
       <c r="C3" s="70"/>
@@ -3070,7 +3070,7 @@
       <c r="Y3" s="71"/>
       <c r="Z3" s="71"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="70"/>
       <c r="B4" s="70"/>
       <c r="C4" s="70"/>
@@ -3098,7 +3098,7 @@
       <c r="Y4" s="71"/>
       <c r="Z4" s="71"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="70"/>
       <c r="B5" s="70"/>
       <c r="C5" s="70"/>
@@ -3126,7 +3126,7 @@
       <c r="Y5" s="71"/>
       <c r="Z5" s="71"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="70"/>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
@@ -3154,7 +3154,7 @@
       <c r="Y6" s="71"/>
       <c r="Z6" s="71"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="70"/>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
@@ -3182,7 +3182,7 @@
       <c r="Y7" s="71"/>
       <c r="Z7" s="71"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="70"/>
       <c r="B8" s="70"/>
       <c r="C8" s="70"/>
@@ -3210,7 +3210,7 @@
       <c r="Y8" s="71"/>
       <c r="Z8" s="71"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="70"/>
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
@@ -3238,7 +3238,7 @@
       <c r="Y9" s="71"/>
       <c r="Z9" s="71"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="70"/>
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
@@ -3266,7 +3266,7 @@
       <c r="Y10" s="71"/>
       <c r="Z10" s="71"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="70"/>
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
@@ -3294,7 +3294,7 @@
       <c r="Y11" s="71"/>
       <c r="Z11" s="71"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="70"/>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
@@ -3322,7 +3322,7 @@
       <c r="Y12" s="71"/>
       <c r="Z12" s="71"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="70"/>
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
@@ -3350,7 +3350,7 @@
       <c r="Y13" s="71"/>
       <c r="Z13" s="71"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="70"/>
       <c r="B14" s="70"/>
       <c r="C14" s="70"/>
@@ -3378,7 +3378,7 @@
       <c r="Y14" s="71"/>
       <c r="Z14" s="71"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="70"/>
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
@@ -3406,7 +3406,7 @@
       <c r="Y15" s="71"/>
       <c r="Z15" s="71"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="86" t="s">
         <v>258</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="Y16" s="71"/>
       <c r="Z16" s="71"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="74"/>
       <c r="B17" s="74"/>
       <c r="C17" s="74"/>
@@ -3464,7 +3464,7 @@
       <c r="Y17" s="71"/>
       <c r="Z17" s="71"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="74"/>
       <c r="B18" s="74"/>
       <c r="C18" s="74"/>
@@ -3492,7 +3492,7 @@
       <c r="Y18" s="71"/>
       <c r="Z18" s="71"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="77" t="s">
         <v>31</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="Y19" s="71"/>
       <c r="Z19" s="71"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="77" t="s">
         <v>259</v>
       </c>
@@ -3556,7 +3556,7 @@
       <c r="Y20" s="71"/>
       <c r="Z20" s="71"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="77" t="s">
         <v>260</v>
       </c>
@@ -3588,7 +3588,7 @@
       <c r="Y21" s="71"/>
       <c r="Z21" s="71"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="77"/>
       <c r="B22" s="80"/>
       <c r="C22" s="80"/>
@@ -3616,7 +3616,7 @@
       <c r="Y22" s="71"/>
       <c r="Z22" s="71"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="77" t="s">
         <v>261</v>
       </c>
@@ -3646,7 +3646,7 @@
       <c r="Y23" s="71"/>
       <c r="Z23" s="71"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="77"/>
       <c r="B24" s="80"/>
       <c r="C24" s="80"/>
@@ -3674,7 +3674,7 @@
       <c r="Y24" s="71"/>
       <c r="Z24" s="71"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="77"/>
       <c r="B25" s="80"/>
       <c r="C25" s="80"/>
@@ -3702,7 +3702,7 @@
       <c r="Y25" s="71"/>
       <c r="Z25" s="71"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="77" t="s">
         <v>262</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="Y26" s="71"/>
       <c r="Z26" s="71"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="77"/>
       <c r="B27" s="80"/>
       <c r="C27" s="80"/>
@@ -3762,7 +3762,7 @@
       <c r="Y27" s="71"/>
       <c r="Z27" s="71"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="77"/>
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
@@ -3790,7 +3790,7 @@
       <c r="Y28" s="71"/>
       <c r="Z28" s="71"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="77" t="s">
         <v>263</v>
       </c>
@@ -3822,7 +3822,7 @@
       <c r="Y29" s="71"/>
       <c r="Z29" s="71"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="77" t="s">
         <v>264</v>
       </c>
@@ -3854,7 +3854,7 @@
       <c r="Y30" s="71"/>
       <c r="Z30" s="71"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="77" t="s">
         <v>266</v>
       </c>
@@ -3886,7 +3886,7 @@
       <c r="Y31" s="71"/>
       <c r="Z31" s="71"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="83"/>
       <c r="B32" s="84" t="s">
         <v>268</v>
@@ -3916,7 +3916,7 @@
       <c r="Y32" s="71"/>
       <c r="Z32" s="71"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="70"/>
       <c r="B33" s="70"/>
       <c r="C33" s="70"/>
@@ -3944,7 +3944,7 @@
       <c r="Y33" s="71"/>
       <c r="Z33" s="71"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="70"/>
       <c r="B34" s="70"/>
       <c r="C34" s="70"/>
@@ -3972,7 +3972,7 @@
       <c r="Y34" s="71"/>
       <c r="Z34" s="71"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="70"/>
       <c r="B35" s="70"/>
       <c r="C35" s="70"/>
@@ -4000,7 +4000,7 @@
       <c r="Y35" s="71"/>
       <c r="Z35" s="71"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="70"/>
       <c r="B36" s="70"/>
       <c r="C36" s="70"/>
@@ -4028,7 +4028,7 @@
       <c r="Y36" s="71"/>
       <c r="Z36" s="71"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="70"/>
       <c r="B37" s="70"/>
       <c r="C37" s="70"/>
@@ -4056,7 +4056,7 @@
       <c r="Y37" s="71"/>
       <c r="Z37" s="71"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="70"/>
       <c r="B38" s="70"/>
       <c r="C38" s="70"/>
@@ -4084,7 +4084,7 @@
       <c r="Y38" s="71"/>
       <c r="Z38" s="71"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="70"/>
       <c r="B39" s="70"/>
       <c r="C39" s="70"/>
@@ -4112,7 +4112,7 @@
       <c r="Y39" s="71"/>
       <c r="Z39" s="71"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="70"/>
       <c r="B40" s="70"/>
       <c r="C40" s="70"/>
@@ -4140,7 +4140,7 @@
       <c r="Y40" s="71"/>
       <c r="Z40" s="71"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="70"/>
       <c r="B41" s="70"/>
       <c r="C41" s="70"/>
@@ -4168,7 +4168,7 @@
       <c r="Y41" s="71"/>
       <c r="Z41" s="71"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="70"/>
       <c r="B42" s="70"/>
       <c r="C42" s="70"/>
@@ -4196,7 +4196,7 @@
       <c r="Y42" s="71"/>
       <c r="Z42" s="71"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="71"/>
       <c r="B43" s="71"/>
       <c r="C43" s="71"/>
@@ -4224,7 +4224,7 @@
       <c r="Y43" s="71"/>
       <c r="Z43" s="71"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="71"/>
       <c r="B44" s="71"/>
       <c r="C44" s="71"/>
@@ -4252,7 +4252,7 @@
       <c r="Y44" s="71"/>
       <c r="Z44" s="71"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="71"/>
       <c r="B45" s="71"/>
       <c r="C45" s="71"/>
@@ -4280,7 +4280,7 @@
       <c r="Y45" s="71"/>
       <c r="Z45" s="71"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="71"/>
       <c r="B46" s="71"/>
       <c r="C46" s="71"/>
@@ -4308,7 +4308,7 @@
       <c r="Y46" s="71"/>
       <c r="Z46" s="71"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="71"/>
       <c r="B47" s="71"/>
       <c r="C47" s="71"/>
@@ -4336,7 +4336,7 @@
       <c r="Y47" s="71"/>
       <c r="Z47" s="71"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="71"/>
       <c r="B48" s="71"/>
       <c r="C48" s="71"/>
@@ -4364,7 +4364,7 @@
       <c r="Y48" s="71"/>
       <c r="Z48" s="71"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="71"/>
       <c r="B49" s="71"/>
       <c r="C49" s="71"/>
@@ -4392,7 +4392,7 @@
       <c r="Y49" s="71"/>
       <c r="Z49" s="71"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="71"/>
       <c r="B50" s="71"/>
       <c r="C50" s="71"/>
@@ -4420,7 +4420,7 @@
       <c r="Y50" s="71"/>
       <c r="Z50" s="71"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="71"/>
       <c r="B51" s="71"/>
       <c r="C51" s="71"/>
@@ -4448,7 +4448,7 @@
       <c r="Y51" s="71"/>
       <c r="Z51" s="71"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="71"/>
       <c r="B52" s="71"/>
       <c r="C52" s="71"/>
@@ -4476,7 +4476,7 @@
       <c r="Y52" s="71"/>
       <c r="Z52" s="71"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="71"/>
       <c r="B53" s="71"/>
       <c r="C53" s="71"/>
@@ -4504,7 +4504,7 @@
       <c r="Y53" s="71"/>
       <c r="Z53" s="71"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="71"/>
       <c r="B54" s="71"/>
       <c r="C54" s="71"/>
@@ -4532,7 +4532,7 @@
       <c r="Y54" s="71"/>
       <c r="Z54" s="71"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="71"/>
       <c r="B55" s="71"/>
       <c r="C55" s="71"/>
@@ -4560,7 +4560,7 @@
       <c r="Y55" s="71"/>
       <c r="Z55" s="71"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="71"/>
       <c r="B56" s="71"/>
       <c r="C56" s="71"/>
@@ -4588,7 +4588,7 @@
       <c r="Y56" s="71"/>
       <c r="Z56" s="71"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="71"/>
       <c r="B57" s="71"/>
       <c r="C57" s="71"/>
@@ -4616,7 +4616,7 @@
       <c r="Y57" s="71"/>
       <c r="Z57" s="71"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="71"/>
       <c r="B58" s="71"/>
       <c r="C58" s="71"/>
@@ -4644,7 +4644,7 @@
       <c r="Y58" s="71"/>
       <c r="Z58" s="71"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="71"/>
       <c r="B59" s="71"/>
       <c r="C59" s="71"/>
@@ -4672,7 +4672,7 @@
       <c r="Y59" s="71"/>
       <c r="Z59" s="71"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="71"/>
       <c r="B60" s="71"/>
       <c r="C60" s="71"/>
@@ -4700,7 +4700,7 @@
       <c r="Y60" s="71"/>
       <c r="Z60" s="71"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="71"/>
       <c r="B61" s="71"/>
       <c r="C61" s="71"/>
@@ -4728,7 +4728,7 @@
       <c r="Y61" s="71"/>
       <c r="Z61" s="71"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="71"/>
       <c r="B62" s="71"/>
       <c r="C62" s="71"/>
@@ -4756,7 +4756,7 @@
       <c r="Y62" s="71"/>
       <c r="Z62" s="71"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="71"/>
       <c r="B63" s="71"/>
       <c r="C63" s="71"/>
@@ -4784,7 +4784,7 @@
       <c r="Y63" s="71"/>
       <c r="Z63" s="71"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="71"/>
       <c r="B64" s="71"/>
       <c r="C64" s="71"/>
@@ -4812,7 +4812,7 @@
       <c r="Y64" s="71"/>
       <c r="Z64" s="71"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="71"/>
       <c r="B65" s="71"/>
       <c r="C65" s="71"/>
@@ -4840,7 +4840,7 @@
       <c r="Y65" s="71"/>
       <c r="Z65" s="71"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="71"/>
       <c r="B66" s="71"/>
       <c r="C66" s="71"/>
@@ -4868,7 +4868,7 @@
       <c r="Y66" s="71"/>
       <c r="Z66" s="71"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="71"/>
       <c r="B67" s="71"/>
       <c r="C67" s="71"/>
@@ -4896,7 +4896,7 @@
       <c r="Y67" s="71"/>
       <c r="Z67" s="71"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="71"/>
       <c r="B68" s="71"/>
       <c r="C68" s="71"/>
@@ -4924,7 +4924,7 @@
       <c r="Y68" s="71"/>
       <c r="Z68" s="71"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="71"/>
       <c r="B69" s="71"/>
       <c r="C69" s="71"/>
@@ -4952,7 +4952,7 @@
       <c r="Y69" s="71"/>
       <c r="Z69" s="71"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="71"/>
       <c r="B70" s="71"/>
       <c r="C70" s="71"/>
@@ -4980,7 +4980,7 @@
       <c r="Y70" s="71"/>
       <c r="Z70" s="71"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="71"/>
       <c r="B71" s="71"/>
       <c r="C71" s="71"/>
@@ -5008,7 +5008,7 @@
       <c r="Y71" s="71"/>
       <c r="Z71" s="71"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="71"/>
       <c r="B72" s="71"/>
       <c r="C72" s="71"/>
@@ -5036,7 +5036,7 @@
       <c r="Y72" s="71"/>
       <c r="Z72" s="71"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="71"/>
       <c r="B73" s="71"/>
       <c r="C73" s="71"/>
@@ -5064,7 +5064,7 @@
       <c r="Y73" s="71"/>
       <c r="Z73" s="71"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="71"/>
       <c r="B74" s="71"/>
       <c r="C74" s="71"/>
@@ -5092,7 +5092,7 @@
       <c r="Y74" s="71"/>
       <c r="Z74" s="71"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="71"/>
       <c r="B75" s="71"/>
       <c r="C75" s="71"/>
@@ -5120,7 +5120,7 @@
       <c r="Y75" s="71"/>
       <c r="Z75" s="71"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="71"/>
       <c r="B76" s="71"/>
       <c r="C76" s="71"/>
@@ -5148,7 +5148,7 @@
       <c r="Y76" s="71"/>
       <c r="Z76" s="71"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="71"/>
       <c r="B77" s="71"/>
       <c r="C77" s="71"/>
@@ -5176,7 +5176,7 @@
       <c r="Y77" s="71"/>
       <c r="Z77" s="71"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="71"/>
       <c r="B78" s="71"/>
       <c r="C78" s="71"/>
@@ -5204,7 +5204,7 @@
       <c r="Y78" s="71"/>
       <c r="Z78" s="71"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="71"/>
       <c r="B79" s="71"/>
       <c r="C79" s="71"/>
@@ -5232,7 +5232,7 @@
       <c r="Y79" s="71"/>
       <c r="Z79" s="71"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="71"/>
       <c r="B80" s="71"/>
       <c r="C80" s="71"/>
@@ -5260,7 +5260,7 @@
       <c r="Y80" s="71"/>
       <c r="Z80" s="71"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="71"/>
       <c r="B81" s="71"/>
       <c r="C81" s="71"/>
@@ -5288,7 +5288,7 @@
       <c r="Y81" s="71"/>
       <c r="Z81" s="71"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="71"/>
       <c r="B82" s="71"/>
       <c r="C82" s="71"/>
@@ -5316,7 +5316,7 @@
       <c r="Y82" s="71"/>
       <c r="Z82" s="71"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="71"/>
       <c r="B83" s="71"/>
       <c r="C83" s="71"/>
@@ -5344,7 +5344,7 @@
       <c r="Y83" s="71"/>
       <c r="Z83" s="71"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="71"/>
       <c r="B84" s="71"/>
       <c r="C84" s="71"/>
@@ -5372,7 +5372,7 @@
       <c r="Y84" s="71"/>
       <c r="Z84" s="71"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="71"/>
       <c r="B85" s="71"/>
       <c r="C85" s="71"/>
@@ -5400,7 +5400,7 @@
       <c r="Y85" s="71"/>
       <c r="Z85" s="71"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="71"/>
       <c r="B86" s="71"/>
       <c r="C86" s="71"/>
@@ -5428,7 +5428,7 @@
       <c r="Y86" s="71"/>
       <c r="Z86" s="71"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="71"/>
       <c r="B87" s="71"/>
       <c r="C87" s="71"/>
@@ -5456,7 +5456,7 @@
       <c r="Y87" s="71"/>
       <c r="Z87" s="71"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="71"/>
       <c r="B88" s="71"/>
       <c r="C88" s="71"/>
@@ -5484,7 +5484,7 @@
       <c r="Y88" s="71"/>
       <c r="Z88" s="71"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="71"/>
       <c r="B89" s="71"/>
       <c r="C89" s="71"/>
@@ -5512,7 +5512,7 @@
       <c r="Y89" s="71"/>
       <c r="Z89" s="71"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="71"/>
       <c r="B90" s="71"/>
       <c r="C90" s="71"/>
@@ -5540,7 +5540,7 @@
       <c r="Y90" s="71"/>
       <c r="Z90" s="71"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="71"/>
       <c r="B91" s="71"/>
       <c r="C91" s="71"/>
@@ -5568,7 +5568,7 @@
       <c r="Y91" s="71"/>
       <c r="Z91" s="71"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="71"/>
       <c r="B92" s="71"/>
       <c r="C92" s="71"/>
@@ -5596,7 +5596,7 @@
       <c r="Y92" s="71"/>
       <c r="Z92" s="71"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="71"/>
       <c r="B93" s="71"/>
       <c r="C93" s="71"/>
@@ -5624,7 +5624,7 @@
       <c r="Y93" s="71"/>
       <c r="Z93" s="71"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="71"/>
       <c r="B94" s="71"/>
       <c r="C94" s="71"/>
@@ -5652,7 +5652,7 @@
       <c r="Y94" s="71"/>
       <c r="Z94" s="71"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="71"/>
       <c r="B95" s="71"/>
       <c r="C95" s="71"/>
@@ -5680,7 +5680,7 @@
       <c r="Y95" s="71"/>
       <c r="Z95" s="71"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="71"/>
       <c r="B96" s="71"/>
       <c r="C96" s="71"/>
@@ -5708,7 +5708,7 @@
       <c r="Y96" s="71"/>
       <c r="Z96" s="71"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="71"/>
       <c r="B97" s="71"/>
       <c r="C97" s="71"/>
@@ -5736,7 +5736,7 @@
       <c r="Y97" s="71"/>
       <c r="Z97" s="71"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="71"/>
       <c r="B98" s="71"/>
       <c r="C98" s="71"/>
@@ -5764,7 +5764,7 @@
       <c r="Y98" s="71"/>
       <c r="Z98" s="71"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="71"/>
       <c r="B99" s="71"/>
       <c r="C99" s="71"/>
@@ -5821,12 +5821,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>2.7466471585410202</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>2.7679848891515602</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>2.7466471585410202</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6208,12 +6208,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>3.22687367398184</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>2.9375514476297502</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>0.48784295359637803</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>0.37305637627958299</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>0.31709791983764601</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>1.2683916793505801</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>43.274952141011099</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>39.394910105381101</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6843,18 +6843,18 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="25" customWidth="1"/>
-    <col min="2" max="3" width="27.28515625" style="25" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="25"/>
-    <col min="7" max="7" width="42.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="56.7109375" style="25" customWidth="1"/>
-    <col min="9" max="9" width="101.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="19.54296875" style="25" customWidth="1"/>
+    <col min="2" max="3" width="27.26953125" style="25" customWidth="1"/>
+    <col min="4" max="6" width="9.1796875" style="25"/>
+    <col min="7" max="7" width="42.7265625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="56.7265625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="101.54296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="25"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
@@ -6865,14 +6865,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="49"/>
       <c r="B5" s="88" t="str">
         <f>"Veda Fill table"</f>
@@ -6880,24 +6880,24 @@
       </c>
       <c r="C5" s="89"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="33"/>
       <c r="B6" s="90" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="91"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="34"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
         <v>52</v>
       </c>
@@ -6906,7 +6906,7 @@
       </c>
       <c r="C9" s="38"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="39" t="s">
         <v>52</v>
       </c>
@@ -6915,21 +6915,21 @@
       </c>
       <c r="C10" s="41"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="42"/>
       <c r="B11" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="42"/>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>57</v>
       </c>
@@ -6940,14 +6940,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>61</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="46" t="s">
         <v>63</v>
       </c>
@@ -6965,14 +6965,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>65</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>67</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>69</v>
       </c>
@@ -6999,14 +6999,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>72</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>74</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>76</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>78</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>80</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>82</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="46" t="s">
         <v>84</v>
       </c>
@@ -7069,14 +7069,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>87</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>11</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
         <v>91</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
         <v>93</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
         <v>95</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="28" t="s">
         <v>97</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
         <v>100</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="28" t="s">
         <v>102</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="28" t="s">
         <v>104</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
         <v>107</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
         <v>109</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="28" t="s">
         <v>112</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
         <v>115</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="28" t="s">
         <v>118</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="46" t="s">
         <v>121</v>
       </c>
@@ -7262,28 +7262,28 @@
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.1796875" style="1"/>
+    <col min="8" max="8" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
@@ -7317,7 +7317,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>S-SH-PU_COA*</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>S-SH-PU_LPG*</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>S-SH-PU_OIL*</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>S-SH-PU_BIO*</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>S-SH-PU_ELC_X0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>S-SH-CS_COA*</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>S-SH-CS_LPG*</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>S-SH-CS_OIL*</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>S-SH-CS_BIO*</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>S-SH-CS_ELC-HP*</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>S-SH-CS_ELC_X0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
         <v>37</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -7779,7 +7779,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>S-WH-PU_SOL*</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>14</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>S-WH-PU_ELC*</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>S-WH-CS_SOL*</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>35</v>
       </c>
@@ -8146,7 +8146,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -8178,7 +8178,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -8210,7 +8210,7 @@
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -8242,7 +8242,7 @@
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -8274,7 +8274,7 @@
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>37</v>
       </c>
@@ -8306,7 +8306,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>37</v>
       </c>
@@ -8339,7 +8339,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>37</v>
       </c>
@@ -8371,7 +8371,7 @@
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -8399,7 +8399,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>37</v>
       </c>
@@ -8511,7 +8511,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>37</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="15" t="s">
         <v>37</v>
       </c>
@@ -8567,7 +8567,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>28</v>
       </c>
@@ -8578,7 +8578,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>14</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -8639,7 +8639,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="15" t="s">
         <v>37</v>
       </c>
@@ -8711,28 +8711,28 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.1796875" style="1"/>
+    <col min="8" max="8" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>S-SH-PU_COA*</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>241</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>S-SH-PU_LPG*</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>241</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>S-SH-PU_OIL*</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>241</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>241</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>S-SH-PU_BIO*</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>241</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>241</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>S-SH-PU_ELC_X0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>241</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>S-SH-CS_COA*</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>241</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>S-SH-CS_LPG*</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>241</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>S-SH-CS_OIL*</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>241</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>241</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>S-SH-CS_BIO*</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>241</v>
       </c>
@@ -9160,7 +9160,7 @@
         <v>S-SH-CS_ELC-HP*</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>241</v>
       </c>
@@ -9189,7 +9189,7 @@
         <v>S-SH-CS_ELC_X0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
         <v>241</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -9228,7 +9228,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>241</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>241</v>
       </c>
@@ -9340,7 +9340,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>241</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>241</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>S-WH-PU_SOL*</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>241</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>S-WH-PU_ELC*</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>241</v>
       </c>
@@ -9480,7 +9480,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -9508,7 +9508,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>241</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>241</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>241</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>S-WH-CS_SOL*</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>241</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>35</v>
       </c>
@@ -9634,7 +9634,7 @@
       <c r="L36" s="17"/>
       <c r="M36" s="17"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -9665,7 +9665,7 @@
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>241</v>
       </c>
@@ -9696,7 +9696,7 @@
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>241</v>
       </c>
@@ -9727,7 +9727,7 @@
       <c r="L39" s="17"/>
       <c r="M39" s="17"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>241</v>
       </c>
@@ -9758,7 +9758,7 @@
       <c r="L40" s="17"/>
       <c r="M40" s="17"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>241</v>
       </c>
@@ -9789,7 +9789,7 @@
       <c r="L41" s="17"/>
       <c r="M41" s="17"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>241</v>
       </c>
@@ -9821,7 +9821,7 @@
       <c r="L42" s="17"/>
       <c r="M42" s="17"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>241</v>
       </c>
@@ -9852,7 +9852,7 @@
       <c r="L43" s="17"/>
       <c r="M43" s="17"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -9880,7 +9880,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>241</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>241</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>241</v>
       </c>
@@ -9964,7 +9964,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>241</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>241</v>
       </c>
@@ -10020,7 +10020,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="15" t="s">
         <v>241</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>28</v>
       </c>
@@ -10059,7 +10059,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>241</v>
       </c>
@@ -10086,7 +10086,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>241</v>
       </c>
@@ -10113,7 +10113,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -10124,7 +10124,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>241</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="15" t="s">
         <v>241</v>
       </c>
@@ -10178,7 +10178,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>254</v>
       </c>
@@ -10189,7 +10189,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>S-REF-PU*</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>127</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>S-REF-CS*</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>127</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>S-OEL-PU*</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>127</v>
       </c>
@@ -10295,7 +10295,7 @@
         <v>S-OEL-CS*</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>127</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>127</v>
       </c>
@@ -10371,7 +10371,7 @@
         <v>9.366584709050458E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>127</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>2.6860059092129972E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="15" t="s">
         <v>127</v>
       </c>
@@ -10457,7 +10457,7 @@
         <v>0.12176560121765607</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>30</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>6.0882800608827838E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>30</v>
       </c>
@@ -10489,7 +10489,7 @@
       <c r="C67" s="7"/>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10509,25 +10509,25 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="1" max="1" width="9.1796875" style="20"/>
     <col min="2" max="2" width="11" style="20" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="20"/>
-    <col min="6" max="6" width="10.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="3" max="3" width="14.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="20"/>
+    <col min="6" max="6" width="10.7265625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>196</v>
       </c>
@@ -10540,7 +10540,7 @@
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="47" t="s">
         <v>16</v>
       </c>
@@ -10590,7 +10590,7 @@
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="47" t="s">
         <v>16</v>
       </c>
@@ -10611,8 +10611,8 @@
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="2:10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>197</v>
       </c>
@@ -10625,7 +10625,7 @@
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="23" t="s">
         <v>15</v>
       </c>
@@ -10654,7 +10654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="47" t="s">
         <v>16</v>
       </c>
@@ -10675,7 +10675,7 @@
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="47" t="s">
         <v>16</v>
       </c>
@@ -10696,8 +10696,8 @@
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
     </row>
-    <row r="12" spans="2:10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>198</v>
       </c>
@@ -10710,7 +10710,7 @@
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="23" t="s">
         <v>15</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="47" t="s">
         <v>16</v>
       </c>
@@ -10760,7 +10760,7 @@
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="47" t="s">
         <v>16</v>
       </c>
@@ -10781,7 +10781,7 @@
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>242</v>
       </c>
@@ -10794,7 +10794,7 @@
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="47" t="s">
         <v>16</v>
       </c>
@@ -10844,7 +10844,7 @@
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="47" t="s">
         <v>16</v>
       </c>
@@ -10880,40 +10880,40 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="50" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="50" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="50" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="3.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.26953125" style="50" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.54296875" style="50" customWidth="1"/>
+    <col min="25" max="25" width="6.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1796875" style="50" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="50" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="50"/>
+    <col min="29" max="29" width="5.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1796875" style="50"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C3" s="51" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -11027,12 +11027,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="50">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="50" t="s">
         <v>128</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="50" t="s">
         <v>131</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="50" t="s">
         <v>132</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="53" t="s">
         <v>133</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="54" t="s">
         <v>135</v>
       </c>
@@ -11397,7 +11397,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="55" t="s">
         <v>137</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
         <v>139</v>
       </c>
@@ -11413,7 +11413,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="55" t="s">
         <v>141</v>
       </c>
@@ -11421,7 +11421,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
         <v>143</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="55" t="s">
         <v>145</v>
       </c>
@@ -11437,7 +11437,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="55" t="s">
         <v>147</v>
       </c>
@@ -11445,7 +11445,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="55" t="s">
         <v>149</v>
       </c>
@@ -11453,7 +11453,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="55" t="s">
         <v>151</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="55" t="s">
         <v>153</v>
       </c>
@@ -11469,7 +11469,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="55" t="s">
         <v>155</v>
       </c>
@@ -11477,7 +11477,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="55" t="s">
         <v>157</v>
       </c>
@@ -11485,7 +11485,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="55" t="s">
         <v>159</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="55" t="s">
         <v>161</v>
       </c>
@@ -11501,7 +11501,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="55" t="s">
         <v>163</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="55" t="s">
         <v>165</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="55" t="s">
         <v>167</v>
       </c>
@@ -11525,7 +11525,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="55" t="s">
         <v>169</v>
       </c>
@@ -11533,7 +11533,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="55" t="s">
         <v>171</v>
       </c>
@@ -11541,7 +11541,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="55" t="s">
         <v>173</v>
       </c>
@@ -11549,7 +11549,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="55" t="s">
         <v>175</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="55" t="s">
         <v>177</v>
       </c>
@@ -11565,7 +11565,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="55" t="s">
         <v>179</v>
       </c>
@@ -11573,7 +11573,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="55" t="s">
         <v>181</v>
       </c>
@@ -11581,7 +11581,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="55" t="s">
         <v>183</v>
       </c>
@@ -11589,7 +11589,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="55" t="s">
         <v>185</v>
       </c>
@@ -11597,7 +11597,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="56" t="s">
         <v>187</v>
       </c>
@@ -11647,44 +11647,44 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="50" customWidth="1"/>
+    <col min="1" max="1" width="2.26953125" style="50" customWidth="1"/>
     <col min="2" max="2" width="10" style="50" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="50" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="2.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="3.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="50"/>
+    <col min="3" max="3" width="23.26953125" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="3.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.453125" style="58" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.26953125" style="58" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="3.453125" style="58" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.453125" style="58" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="2.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.26953125" style="58" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.453125" style="58" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.26953125" style="58" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="3.26953125" style="50" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.7265625" style="50" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.1796875" style="50"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B3" s="57" t="s">
         <v>188</v>
       </c>
@@ -11708,7 +11708,7 @@
       <c r="Z3" s="50"/>
       <c r="AA3" s="50"/>
     </row>
-    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="60" t="s">
         <v>189</v>
       </c>
@@ -11754,7 +11754,7 @@
       <c r="Z4" s="50"/>
       <c r="AA4" s="50"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
       <c r="C5" s="63" t="s">
         <v>30</v>
       </c>
@@ -11786,7 +11786,7 @@
       <c r="Z5" s="50"/>
       <c r="AA5" s="50"/>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
       <c r="J6" s="50"/>
       <c r="K6" s="50"/>
       <c r="L6" s="50"/>
@@ -11806,7 +11806,7 @@
       <c r="Z6" s="50"/>
       <c r="AA6" s="50"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>
@@ -11842,12 +11842,12 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -11888,7 +11888,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -11970,7 +11970,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -12011,7 +12011,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -12093,7 +12093,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -12175,7 +12175,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -12257,7 +12257,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -12380,7 +12380,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -12421,7 +12421,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -12462,7 +12462,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -12503,7 +12503,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -12544,7 +12544,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -12585,7 +12585,7 @@
         <v>0.63490443337371305</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -12626,7 +12626,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -12667,7 +12667,7 @@
         <v>2.74705437385472</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>0.81595511259153497</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>0.77299617086321304</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -12790,7 +12790,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -12831,7 +12831,7 @@
         <v>0.65835584489725196</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -12913,7 +12913,7 @@
         <v>0.63490443337371305</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>2.74705437385472</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>0.81595511259153497</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -13077,7 +13077,7 @@
         <v>0.77299617086321304</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>0.65835584489725196</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -13215,12 +13215,12 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -13261,7 +13261,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -13343,7 +13343,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -13384,7 +13384,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -13507,7 +13507,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -13630,7 +13630,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -13712,7 +13712,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -13753,7 +13753,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -13835,7 +13835,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -13876,7 +13876,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -13917,7 +13917,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -13958,7 +13958,7 @@
         <v>0.77915338816094504</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -13999,7 +13999,7 @@
         <v>0.63024757853709501</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -14040,7 +14040,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>0.59834963673469899</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -14122,7 +14122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -14163,7 +14163,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -14245,7 +14245,7 @@
         <v>0.77915338816094504</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -14286,7 +14286,7 @@
         <v>0.63024757853709501</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -14327,7 +14327,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>0.59834963673469899</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Service DH Flow issue
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C3A4C4-5EB5-4E0C-88FC-C9BAA49A9B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1D1E7D-7258-4815-BB38-59630E822859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="19" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="BY_S-SC" sheetId="11" r:id="rId10"/>
     <sheet name="BY_S-EAP" sheetId="18" r:id="rId11"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId12"/>
+  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="6" hidden="1">#REF!</definedName>
@@ -542,7 +545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="273">
   <si>
     <t>LimType</t>
   </si>
@@ -2177,7 +2180,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF08F70-6061-4334-B6F9-12A767772C59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2224,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CE3B6C-F45A-4A9A-83A7-260FE2022E45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2270,7 +2273,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F6629FB-C09F-4200-B78E-4FD5614996BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2323,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA8B95B-A935-4706-BBFB-6D5C157F61C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2370,7 +2373,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DB6255-16F1-4131-B80B-898A983DA66E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2419,7 +2422,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C8A817-8A7F-451D-A8EF-15CA92E73ED5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -2481,7 +2484,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1104FA2-617F-40B5-9110-C12C45401468}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2536,7 +2539,7 @@
         <xdr:cNvPr id="2" name="Arrow: Right 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2642,6 +2645,29 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Regions"/>
+      <sheetName val="TechSelection"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2968,7 +2994,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -7258,7 +7284,7 @@
   </sheetPr>
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
@@ -11641,10 +11667,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB4249C-0490-477F-A930-E3E0809B104E}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B3:AA7"/>
+  <dimension ref="B3:AH7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11684,7 +11710,7 @@
     <col min="38" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" s="57" t="s">
         <v>188</v>
       </c>
@@ -11708,7 +11734,7 @@
       <c r="Z3" s="50"/>
       <c r="AA3" s="50"/>
     </row>
-    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="60" t="s">
         <v>189</v>
       </c>
@@ -11728,33 +11754,89 @@
         <v>193</v>
       </c>
       <c r="H4" s="61" t="str">
-        <f>Regions!C3</f>
+        <f>[1]Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="I4" s="62" t="str">
-        <f>Regions!D3</f>
-        <v>National</v>
-      </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I4" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="K4" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="P4" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q4" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="R4" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="S4" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="T4" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="U4" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="V4" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="W4" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="X4" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y4" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z4" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA4" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB4" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC4" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD4" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE4" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="AF4" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG4" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH4" s="62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C5" s="63" t="s">
         <v>30</v>
       </c>
@@ -11764,29 +11846,86 @@
       <c r="H5" s="50">
         <v>1</v>
       </c>
-      <c r="I5" s="59">
+      <c r="I5" s="50">
         <v>1</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="J5" s="50">
+        <v>1</v>
+      </c>
+      <c r="K5" s="50">
+        <v>1</v>
+      </c>
+      <c r="L5" s="50">
+        <v>1</v>
+      </c>
+      <c r="M5" s="50">
+        <v>1</v>
+      </c>
+      <c r="N5" s="50">
+        <v>1</v>
+      </c>
+      <c r="O5" s="50">
+        <v>1</v>
+      </c>
+      <c r="P5" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="50">
+        <v>1</v>
+      </c>
+      <c r="R5" s="50">
+        <v>1</v>
+      </c>
+      <c r="S5" s="50">
+        <v>1</v>
+      </c>
+      <c r="T5" s="50">
+        <v>1</v>
+      </c>
+      <c r="U5" s="50">
+        <v>1</v>
+      </c>
+      <c r="V5" s="50">
+        <v>1</v>
+      </c>
+      <c r="W5" s="50">
+        <v>1</v>
+      </c>
+      <c r="X5" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="50">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="50">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="J6" s="50"/>
       <c r="K6" s="50"/>
       <c r="L6" s="50"/>
@@ -11806,7 +11945,7 @@
       <c r="Z6" s="50"/>
       <c r="AA6" s="50"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>

</xml_diff>

<commit_message>
CB_overshoot run version eith case definitions
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91D2BE-AD7F-43B2-94CD-F8799C205949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76369195-50C6-49C0-84CA-D86EE33ACA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="1815" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="19" r:id="rId1"/>
@@ -2565,7 +2565,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2943,20 +2943,20 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.6328125" customWidth="1"/>
-    <col min="5" max="6" width="14.08984375" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
-    <col min="8" max="10" width="8.08984375" customWidth="1"/>
-    <col min="11" max="11" width="9.6328125" customWidth="1"/>
-    <col min="12" max="12" width="8.08984375" customWidth="1"/>
+    <col min="1" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" customWidth="1"/>
-    <col min="15" max="15" width="13.453125" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="59"/>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2984,7 +2984,7 @@
       <c r="Y1" s="60"/>
       <c r="Z1" s="60"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -3012,7 +3012,7 @@
       <c r="Y2" s="60"/>
       <c r="Z2" s="60"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -3040,7 +3040,7 @@
       <c r="Y3" s="60"/>
       <c r="Z3" s="60"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -3068,7 +3068,7 @@
       <c r="Y4" s="60"/>
       <c r="Z4" s="60"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="59"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -3096,7 +3096,7 @@
       <c r="Y5" s="60"/>
       <c r="Z5" s="60"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -3124,7 +3124,7 @@
       <c r="Y6" s="60"/>
       <c r="Z6" s="60"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -3152,7 +3152,7 @@
       <c r="Y7" s="60"/>
       <c r="Z7" s="60"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3180,7 +3180,7 @@
       <c r="Y8" s="60"/>
       <c r="Z8" s="60"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -3208,7 +3208,7 @@
       <c r="Y9" s="60"/>
       <c r="Z9" s="60"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -3236,7 +3236,7 @@
       <c r="Y10" s="60"/>
       <c r="Z10" s="60"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="59"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -3264,7 +3264,7 @@
       <c r="Y11" s="60"/>
       <c r="Z11" s="60"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="59"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -3292,7 +3292,7 @@
       <c r="Y12" s="60"/>
       <c r="Z12" s="60"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="59"/>
       <c r="B13" s="59"/>
       <c r="C13" s="59"/>
@@ -3320,7 +3320,7 @@
       <c r="Y13" s="60"/>
       <c r="Z13" s="60"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="59"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -3348,7 +3348,7 @@
       <c r="Y14" s="60"/>
       <c r="Z14" s="60"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -3376,7 +3376,7 @@
       <c r="Y15" s="60"/>
       <c r="Z15" s="60"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
         <v>258</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="Y16" s="60"/>
       <c r="Z16" s="60"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
       <c r="B17" s="63"/>
       <c r="C17" s="63"/>
@@ -3434,7 +3434,7 @@
       <c r="Y17" s="60"/>
       <c r="Z17" s="60"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="63"/>
       <c r="B18" s="63"/>
       <c r="C18" s="63"/>
@@ -3462,7 +3462,7 @@
       <c r="Y18" s="60"/>
       <c r="Z18" s="60"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
         <v>31</v>
       </c>
@@ -3494,7 +3494,7 @@
       <c r="Y19" s="60"/>
       <c r="Z19" s="60"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
         <v>259</v>
       </c>
@@ -3526,7 +3526,7 @@
       <c r="Y20" s="60"/>
       <c r="Z20" s="60"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
         <v>260</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="Y21" s="60"/>
       <c r="Z21" s="60"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="66"/>
       <c r="B22" s="69"/>
       <c r="C22" s="69"/>
@@ -3586,7 +3586,7 @@
       <c r="Y22" s="60"/>
       <c r="Z22" s="60"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
         <v>261</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="Y23" s="60"/>
       <c r="Z23" s="60"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="66"/>
       <c r="B24" s="69"/>
       <c r="C24" s="69"/>
@@ -3644,7 +3644,7 @@
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="66"/>
       <c r="B25" s="69"/>
       <c r="C25" s="69"/>
@@ -3672,7 +3672,7 @@
       <c r="Y25" s="60"/>
       <c r="Z25" s="60"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
         <v>262</v>
       </c>
@@ -3704,7 +3704,7 @@
       <c r="Y26" s="60"/>
       <c r="Z26" s="60"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="66"/>
       <c r="B27" s="69"/>
       <c r="C27" s="69"/>
@@ -3732,7 +3732,7 @@
       <c r="Y27" s="60"/>
       <c r="Z27" s="60"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
       <c r="B28" s="69"/>
       <c r="C28" s="69"/>
@@ -3760,7 +3760,7 @@
       <c r="Y28" s="60"/>
       <c r="Z28" s="60"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="66" t="s">
         <v>263</v>
       </c>
@@ -3792,7 +3792,7 @@
       <c r="Y29" s="60"/>
       <c r="Z29" s="60"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="66" t="s">
         <v>264</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="Y30" s="60"/>
       <c r="Z30" s="60"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="66" t="s">
         <v>266</v>
       </c>
@@ -3856,7 +3856,7 @@
       <c r="Y31" s="60"/>
       <c r="Z31" s="60"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="72"/>
       <c r="B32" s="73" t="s">
         <v>268</v>
@@ -3886,7 +3886,7 @@
       <c r="Y32" s="60"/>
       <c r="Z32" s="60"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="59"/>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -3914,7 +3914,7 @@
       <c r="Y33" s="60"/>
       <c r="Z33" s="60"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="59"/>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
@@ -3942,7 +3942,7 @@
       <c r="Y34" s="60"/>
       <c r="Z34" s="60"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="59"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -3970,7 +3970,7 @@
       <c r="Y35" s="60"/>
       <c r="Z35" s="60"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="59"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -3998,7 +3998,7 @@
       <c r="Y36" s="60"/>
       <c r="Z36" s="60"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="59"/>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -4026,7 +4026,7 @@
       <c r="Y37" s="60"/>
       <c r="Z37" s="60"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="59"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -4054,7 +4054,7 @@
       <c r="Y38" s="60"/>
       <c r="Z38" s="60"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="59"/>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -4082,7 +4082,7 @@
       <c r="Y39" s="60"/>
       <c r="Z39" s="60"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="59"/>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -4110,7 +4110,7 @@
       <c r="Y40" s="60"/>
       <c r="Z40" s="60"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
       <c r="B41" s="59"/>
       <c r="C41" s="59"/>
@@ -4138,7 +4138,7 @@
       <c r="Y41" s="60"/>
       <c r="Z41" s="60"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -4166,7 +4166,7 @@
       <c r="Y42" s="60"/>
       <c r="Z42" s="60"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
       <c r="C43" s="60"/>
@@ -4194,7 +4194,7 @@
       <c r="Y43" s="60"/>
       <c r="Z43" s="60"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
       <c r="C44" s="60"/>
@@ -4222,7 +4222,7 @@
       <c r="Y44" s="60"/>
       <c r="Z44" s="60"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="60"/>
       <c r="B45" s="60"/>
       <c r="C45" s="60"/>
@@ -4250,7 +4250,7 @@
       <c r="Y45" s="60"/>
       <c r="Z45" s="60"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="60"/>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
@@ -4278,7 +4278,7 @@
       <c r="Y46" s="60"/>
       <c r="Z46" s="60"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="60"/>
       <c r="B47" s="60"/>
       <c r="C47" s="60"/>
@@ -4306,7 +4306,7 @@
       <c r="Y47" s="60"/>
       <c r="Z47" s="60"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="60"/>
       <c r="B48" s="60"/>
       <c r="C48" s="60"/>
@@ -4334,7 +4334,7 @@
       <c r="Y48" s="60"/>
       <c r="Z48" s="60"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="60"/>
       <c r="B49" s="60"/>
       <c r="C49" s="60"/>
@@ -4362,7 +4362,7 @@
       <c r="Y49" s="60"/>
       <c r="Z49" s="60"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="60"/>
       <c r="B50" s="60"/>
       <c r="C50" s="60"/>
@@ -4390,7 +4390,7 @@
       <c r="Y50" s="60"/>
       <c r="Z50" s="60"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="60"/>
       <c r="B51" s="60"/>
       <c r="C51" s="60"/>
@@ -4418,7 +4418,7 @@
       <c r="Y51" s="60"/>
       <c r="Z51" s="60"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="60"/>
       <c r="B52" s="60"/>
       <c r="C52" s="60"/>
@@ -4446,7 +4446,7 @@
       <c r="Y52" s="60"/>
       <c r="Z52" s="60"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="60"/>
       <c r="B53" s="60"/>
       <c r="C53" s="60"/>
@@ -4474,7 +4474,7 @@
       <c r="Y53" s="60"/>
       <c r="Z53" s="60"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="60"/>
       <c r="B54" s="60"/>
       <c r="C54" s="60"/>
@@ -4502,7 +4502,7 @@
       <c r="Y54" s="60"/>
       <c r="Z54" s="60"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="60"/>
       <c r="B55" s="60"/>
       <c r="C55" s="60"/>
@@ -4530,7 +4530,7 @@
       <c r="Y55" s="60"/>
       <c r="Z55" s="60"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="60"/>
       <c r="B56" s="60"/>
       <c r="C56" s="60"/>
@@ -4558,7 +4558,7 @@
       <c r="Y56" s="60"/>
       <c r="Z56" s="60"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="60"/>
       <c r="B57" s="60"/>
       <c r="C57" s="60"/>
@@ -4586,7 +4586,7 @@
       <c r="Y57" s="60"/>
       <c r="Z57" s="60"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="60"/>
       <c r="B58" s="60"/>
       <c r="C58" s="60"/>
@@ -4614,7 +4614,7 @@
       <c r="Y58" s="60"/>
       <c r="Z58" s="60"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
       <c r="B59" s="60"/>
       <c r="C59" s="60"/>
@@ -4642,7 +4642,7 @@
       <c r="Y59" s="60"/>
       <c r="Z59" s="60"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="60"/>
       <c r="B60" s="60"/>
       <c r="C60" s="60"/>
@@ -4670,7 +4670,7 @@
       <c r="Y60" s="60"/>
       <c r="Z60" s="60"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="B61" s="60"/>
       <c r="C61" s="60"/>
@@ -4698,7 +4698,7 @@
       <c r="Y61" s="60"/>
       <c r="Z61" s="60"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="60"/>
       <c r="B62" s="60"/>
       <c r="C62" s="60"/>
@@ -4726,7 +4726,7 @@
       <c r="Y62" s="60"/>
       <c r="Z62" s="60"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="60"/>
       <c r="B63" s="60"/>
       <c r="C63" s="60"/>
@@ -4754,7 +4754,7 @@
       <c r="Y63" s="60"/>
       <c r="Z63" s="60"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="60"/>
       <c r="B64" s="60"/>
       <c r="C64" s="60"/>
@@ -4782,7 +4782,7 @@
       <c r="Y64" s="60"/>
       <c r="Z64" s="60"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="60"/>
       <c r="B65" s="60"/>
       <c r="C65" s="60"/>
@@ -4810,7 +4810,7 @@
       <c r="Y65" s="60"/>
       <c r="Z65" s="60"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="60"/>
       <c r="B66" s="60"/>
       <c r="C66" s="60"/>
@@ -4838,7 +4838,7 @@
       <c r="Y66" s="60"/>
       <c r="Z66" s="60"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="60"/>
       <c r="B67" s="60"/>
       <c r="C67" s="60"/>
@@ -4866,7 +4866,7 @@
       <c r="Y67" s="60"/>
       <c r="Z67" s="60"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="60"/>
       <c r="B68" s="60"/>
       <c r="C68" s="60"/>
@@ -4894,7 +4894,7 @@
       <c r="Y68" s="60"/>
       <c r="Z68" s="60"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="60"/>
       <c r="B69" s="60"/>
       <c r="C69" s="60"/>
@@ -4922,7 +4922,7 @@
       <c r="Y69" s="60"/>
       <c r="Z69" s="60"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="60"/>
       <c r="B70" s="60"/>
       <c r="C70" s="60"/>
@@ -4950,7 +4950,7 @@
       <c r="Y70" s="60"/>
       <c r="Z70" s="60"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="60"/>
       <c r="B71" s="60"/>
       <c r="C71" s="60"/>
@@ -4978,7 +4978,7 @@
       <c r="Y71" s="60"/>
       <c r="Z71" s="60"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="60"/>
       <c r="B72" s="60"/>
       <c r="C72" s="60"/>
@@ -5006,7 +5006,7 @@
       <c r="Y72" s="60"/>
       <c r="Z72" s="60"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="60"/>
       <c r="B73" s="60"/>
       <c r="C73" s="60"/>
@@ -5034,7 +5034,7 @@
       <c r="Y73" s="60"/>
       <c r="Z73" s="60"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="60"/>
       <c r="B74" s="60"/>
       <c r="C74" s="60"/>
@@ -5062,7 +5062,7 @@
       <c r="Y74" s="60"/>
       <c r="Z74" s="60"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="60"/>
       <c r="B75" s="60"/>
       <c r="C75" s="60"/>
@@ -5090,7 +5090,7 @@
       <c r="Y75" s="60"/>
       <c r="Z75" s="60"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="60"/>
       <c r="B76" s="60"/>
       <c r="C76" s="60"/>
@@ -5118,7 +5118,7 @@
       <c r="Y76" s="60"/>
       <c r="Z76" s="60"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="60"/>
       <c r="B77" s="60"/>
       <c r="C77" s="60"/>
@@ -5146,7 +5146,7 @@
       <c r="Y77" s="60"/>
       <c r="Z77" s="60"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="60"/>
       <c r="B78" s="60"/>
       <c r="C78" s="60"/>
@@ -5174,7 +5174,7 @@
       <c r="Y78" s="60"/>
       <c r="Z78" s="60"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="60"/>
       <c r="B79" s="60"/>
       <c r="C79" s="60"/>
@@ -5202,7 +5202,7 @@
       <c r="Y79" s="60"/>
       <c r="Z79" s="60"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="60"/>
       <c r="B80" s="60"/>
       <c r="C80" s="60"/>
@@ -5230,7 +5230,7 @@
       <c r="Y80" s="60"/>
       <c r="Z80" s="60"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="60"/>
       <c r="B81" s="60"/>
       <c r="C81" s="60"/>
@@ -5258,7 +5258,7 @@
       <c r="Y81" s="60"/>
       <c r="Z81" s="60"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="60"/>
       <c r="B82" s="60"/>
       <c r="C82" s="60"/>
@@ -5286,7 +5286,7 @@
       <c r="Y82" s="60"/>
       <c r="Z82" s="60"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="60"/>
       <c r="B83" s="60"/>
       <c r="C83" s="60"/>
@@ -5314,7 +5314,7 @@
       <c r="Y83" s="60"/>
       <c r="Z83" s="60"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="60"/>
       <c r="B84" s="60"/>
       <c r="C84" s="60"/>
@@ -5342,7 +5342,7 @@
       <c r="Y84" s="60"/>
       <c r="Z84" s="60"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="60"/>
       <c r="B85" s="60"/>
       <c r="C85" s="60"/>
@@ -5370,7 +5370,7 @@
       <c r="Y85" s="60"/>
       <c r="Z85" s="60"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="60"/>
       <c r="B86" s="60"/>
       <c r="C86" s="60"/>
@@ -5398,7 +5398,7 @@
       <c r="Y86" s="60"/>
       <c r="Z86" s="60"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="60"/>
       <c r="B87" s="60"/>
       <c r="C87" s="60"/>
@@ -5426,7 +5426,7 @@
       <c r="Y87" s="60"/>
       <c r="Z87" s="60"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="60"/>
       <c r="B88" s="60"/>
       <c r="C88" s="60"/>
@@ -5454,7 +5454,7 @@
       <c r="Y88" s="60"/>
       <c r="Z88" s="60"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="60"/>
       <c r="B89" s="60"/>
       <c r="C89" s="60"/>
@@ -5482,7 +5482,7 @@
       <c r="Y89" s="60"/>
       <c r="Z89" s="60"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="60"/>
       <c r="B90" s="60"/>
       <c r="C90" s="60"/>
@@ -5510,7 +5510,7 @@
       <c r="Y90" s="60"/>
       <c r="Z90" s="60"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="60"/>
       <c r="B91" s="60"/>
       <c r="C91" s="60"/>
@@ -5538,7 +5538,7 @@
       <c r="Y91" s="60"/>
       <c r="Z91" s="60"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="60"/>
       <c r="B92" s="60"/>
       <c r="C92" s="60"/>
@@ -5566,7 +5566,7 @@
       <c r="Y92" s="60"/>
       <c r="Z92" s="60"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="60"/>
       <c r="B93" s="60"/>
       <c r="C93" s="60"/>
@@ -5594,7 +5594,7 @@
       <c r="Y93" s="60"/>
       <c r="Z93" s="60"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="60"/>
       <c r="B94" s="60"/>
       <c r="C94" s="60"/>
@@ -5622,7 +5622,7 @@
       <c r="Y94" s="60"/>
       <c r="Z94" s="60"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="60"/>
       <c r="B95" s="60"/>
       <c r="C95" s="60"/>
@@ -5650,7 +5650,7 @@
       <c r="Y95" s="60"/>
       <c r="Z95" s="60"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="60"/>
       <c r="B96" s="60"/>
       <c r="C96" s="60"/>
@@ -5678,7 +5678,7 @@
       <c r="Y96" s="60"/>
       <c r="Z96" s="60"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="60"/>
       <c r="B97" s="60"/>
       <c r="C97" s="60"/>
@@ -5706,7 +5706,7 @@
       <c r="Y97" s="60"/>
       <c r="Z97" s="60"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="60"/>
       <c r="B98" s="60"/>
       <c r="C98" s="60"/>
@@ -5734,7 +5734,7 @@
       <c r="Y98" s="60"/>
       <c r="Z98" s="60"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="60"/>
       <c r="B99" s="60"/>
       <c r="C99" s="60"/>
@@ -5791,12 +5791,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>3.42465753424658E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>2.7466471585410202</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>2.7679848891515602</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>2.7466471585410202</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6178,12 +6178,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>2.5559498489728498</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>4.0979523881676903</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>0.48784295359637803</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>0.37305637627958299</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>0.31709791983764601</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>1.2683916793505801</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>34.2773280159549</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>54.9568131234806</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6813,16 +6813,16 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="2" max="3" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="42.6328125" customWidth="1"/>
-    <col min="8" max="8" width="56.6328125" customWidth="1"/>
-    <col min="9" max="9" width="101.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
+    <col min="8" max="8" width="56.5703125" customWidth="1"/>
+    <col min="9" max="9" width="101.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>32</v>
       </c>
@@ -6833,14 +6833,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
       <c r="B5" s="77" t="str">
         <f>"Veda Fill table"</f>
@@ -6848,24 +6848,24 @@
       </c>
       <c r="C5" s="78"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
       <c r="B6" s="79" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="80"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
     </row>
-    <row r="8" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>52</v>
       </c>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="C9" s="32"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>52</v>
       </c>
@@ -6883,19 +6883,19 @@
       </c>
       <c r="C10" s="35"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="31" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="36"/>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>57</v>
       </c>
@@ -6906,14 +6906,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>63</v>
       </c>
@@ -6931,14 +6931,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
@@ -6965,14 +6965,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>84</v>
       </c>
@@ -7035,12 +7035,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>97</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>100</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>102</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>104</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>107</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>109</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>118</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>121</v>
       </c>
@@ -7226,28 +7226,28 @@
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.08984375" style="1"/>
-    <col min="8" max="8" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="1"/>
+    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>26</v>
       </c>
@@ -7281,7 +7281,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>S-SH-PU_COA*</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>S-SH-PU_LPG*</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>S-SH-PU_OIL*</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>S-SH-PU_BIO*</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>S-SH-PU_ELC_X0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>S-SH-CS_COA*</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>S-SH-CS_LPG*</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>S-SH-CS_OIL*</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>S-SH-CS_BIO*</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>S-SH-CS_ELC-HP*</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>S-SH-CS_ELC_X0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>37</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>27</v>
       </c>
@@ -7740,7 +7740,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>S-WH-PU_SOL*</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>14</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>S-WH-PU_ELC*</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -7991,7 +7991,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>S-WH-CS_SOL*</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
@@ -8103,7 +8103,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>S-WH-PU_ELC*</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>37</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -8383,7 +8383,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>37</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>37</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>28</v>
       </c>
@@ -8506,7 +8506,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>14</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>36</v>
       </c>
@@ -8566,7 +8566,7 @@
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>37</v>
       </c>
@@ -8638,28 +8638,28 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.08984375" style="1"/>
-    <col min="8" max="8" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>26</v>
       </c>
@@ -8693,7 +8693,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>S-SH-PU_COA*</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>241</v>
       </c>
@@ -8749,7 +8749,7 @@
         <v>S-SH-PU_LPG*</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>241</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>S-SH-PU_OIL*</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>241</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>241</v>
       </c>
@@ -8833,7 +8833,7 @@
         <v>S-SH-PU_BIO*</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>241</v>
       </c>
@@ -8861,7 +8861,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>241</v>
       </c>
@@ -8889,7 +8889,7 @@
         <v>S-SH-PU_ELC_X0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>241</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>S-SH-PU_GAS*</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>S-SH-CS_COA*</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>241</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>S-SH-CS_LPG*</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>241</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>S-SH-CS_OIL*</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>241</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>241</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>S-SH-CS_BIO*</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>241</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>S-SH-CS_ELC-HP*</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>241</v>
       </c>
@@ -9113,7 +9113,7 @@
         <v>S-SH-CS_ELC_X0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>241</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>S-SH-CS_GAS*</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>27</v>
       </c>
@@ -9152,7 +9152,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>241</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>241</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>241</v>
       </c>
@@ -9292,7 +9292,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>241</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>S-WH-PU_SOL*</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>241</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>S-WH-PU_ELC*</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>241</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>241</v>
       </c>
@@ -9460,7 +9460,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>241</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>241</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>S-WH-CS_SOL*</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>241</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>S-WH-CS_ELC*</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>35</v>
       </c>
@@ -9555,7 +9555,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>S-WH-PU_COA*</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>241</v>
       </c>
@@ -9611,7 +9611,7 @@
         <v>S-WH-PU_LPG*</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>241</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>S-WH-PU_OIL*</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>241</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>241</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>S-WH-PU_BIO*</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>241</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>241</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>S-WH-PU_GAS*</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>S-WH-CS_COA*</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>241</v>
       </c>
@@ -9807,7 +9807,7 @@
         <v>S-WH-CS_LPG*</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>241</v>
       </c>
@@ -9835,7 +9835,7 @@
         <v>S-WH-CS_OIL*</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>241</v>
       </c>
@@ -9863,7 +9863,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>241</v>
       </c>
@@ -9891,7 +9891,7 @@
         <v>S-WH-CS_BIO*</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>241</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>S-SH-PU_ELC-HP*</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>241</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>S-WH-CS_GAS*</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>28</v>
       </c>
@@ -9958,7 +9958,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>241</v>
       </c>
@@ -9985,7 +9985,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>241</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>36</v>
       </c>
@@ -10023,7 +10023,7 @@
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>241</v>
       </c>
@@ -10050,7 +10050,7 @@
         <v>S-SC-PU_ELC*</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>241</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>S-SC-CS_ELC*</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>254</v>
       </c>
@@ -10088,7 +10088,7 @@
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
@@ -10113,7 +10113,7 @@
         <v>S-REF-PU*</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>127</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>S-REF-CS*</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>127</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>S-OEL-PU*</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>127</v>
       </c>
@@ -10188,7 +10188,7 @@
         <v>S-OEL-CS*</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>9.366584709050458E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>127</v>
       </c>
@@ -10301,7 +10301,7 @@
         <v>2.6860059092129972E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>127</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>0.12176560121765607</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>30</v>
       </c>
@@ -10364,7 +10364,7 @@
         <v>6.0882800608827838E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>30</v>
       </c>
@@ -10388,25 +10388,25 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
     <col min="2" max="2" width="11" style="16" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="16"/>
-    <col min="6" max="6" width="10.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="16"/>
+    <col min="3" max="3" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="16"/>
+    <col min="6" max="6" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>196</v>
       </c>
@@ -10419,7 +10419,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
         <v>15</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>16</v>
       </c>
@@ -10469,7 +10469,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>16</v>
       </c>
@@ -10490,8 +10490,8 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="2:10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>197</v>
       </c>
@@ -10504,7 +10504,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>15</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>16</v>
       </c>
@@ -10554,7 +10554,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
@@ -10575,8 +10575,8 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="2:10" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>198</v>
       </c>
@@ -10589,7 +10589,7 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
     </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>15</v>
       </c>
@@ -10618,7 +10618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>16</v>
       </c>
@@ -10639,7 +10639,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -10660,7 +10660,7 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>242</v>
       </c>
@@ -10673,7 +10673,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>16</v>
       </c>
@@ -10723,7 +10723,7 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>16</v>
       </c>
@@ -10759,39 +10759,37 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="3.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" customWidth="1"/>
-    <col min="25" max="25" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="41" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -10905,12 +10903,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -11025,7 +11023,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -11142,7 +11140,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -11259,7 +11257,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
         <v>133</v>
       </c>
@@ -11267,7 +11265,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>135</v>
       </c>
@@ -11275,7 +11273,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>137</v>
       </c>
@@ -11283,7 +11281,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>139</v>
       </c>
@@ -11291,7 +11289,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
         <v>141</v>
       </c>
@@ -11299,7 +11297,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>143</v>
       </c>
@@ -11307,7 +11305,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>145</v>
       </c>
@@ -11315,7 +11313,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>147</v>
       </c>
@@ -11323,7 +11321,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>149</v>
       </c>
@@ -11331,7 +11329,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>151</v>
       </c>
@@ -11339,7 +11337,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
         <v>153</v>
       </c>
@@ -11347,7 +11345,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
         <v>155</v>
       </c>
@@ -11355,7 +11353,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
         <v>157</v>
       </c>
@@ -11363,7 +11361,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
         <v>159</v>
       </c>
@@ -11371,7 +11369,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
         <v>161</v>
       </c>
@@ -11379,7 +11377,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
         <v>163</v>
       </c>
@@ -11387,7 +11385,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
         <v>165</v>
       </c>
@@ -11395,7 +11393,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
         <v>167</v>
       </c>
@@ -11403,7 +11401,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
         <v>169</v>
       </c>
@@ -11411,7 +11409,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
         <v>171</v>
       </c>
@@ -11419,7 +11417,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
         <v>173</v>
       </c>
@@ -11427,7 +11425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
         <v>175</v>
       </c>
@@ -11435,7 +11433,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
         <v>177</v>
       </c>
@@ -11443,7 +11441,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
         <v>179</v>
       </c>
@@ -11451,7 +11449,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
         <v>181</v>
       </c>
@@ -11459,7 +11457,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="45" t="s">
         <v>183</v>
       </c>
@@ -11467,7 +11465,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
         <v>185</v>
       </c>
@@ -11475,7 +11473,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
         <v>187</v>
       </c>
@@ -11501,7 +11499,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -11525,43 +11523,37 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.36328125" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="2.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.54296875" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.36328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.54296875" style="48" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.54296875" style="48" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="2.6328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.54296875" style="48" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.36328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.36328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.6328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="3.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="3.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="2.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="3.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="47" t="s">
         <v>188</v>
       </c>
@@ -11585,7 +11577,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>189</v>
       </c>
@@ -11631,7 +11623,7 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C5" s="53" t="s">
         <v>30</v>
       </c>
@@ -11663,7 +11655,7 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -11683,7 +11675,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -11719,12 +11711,12 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -11765,7 +11757,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11806,7 +11798,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -11847,7 +11839,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -11888,7 +11880,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -11929,7 +11921,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -11970,7 +11962,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -12011,7 +12003,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -12052,7 +12044,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -12093,7 +12085,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -12134,7 +12126,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -12175,7 +12167,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -12216,7 +12208,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -12257,7 +12249,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -12298,7 +12290,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -12339,7 +12331,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -12380,7 +12372,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -12421,7 +12413,7 @@
         <v>0.114155251141553</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -12462,7 +12454,7 @@
         <v>0.63490443337371305</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -12503,7 +12495,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -12544,7 +12536,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -12585,7 +12577,7 @@
         <v>0.81595511259153497</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -12626,7 +12618,7 @@
         <v>0.77299617086321304</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -12667,7 +12659,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -12708,7 +12700,7 @@
         <v>0.65835584489725196</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -12749,7 +12741,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -12790,7 +12782,7 @@
         <v>0.63490443337371305</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -12831,7 +12823,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -12872,7 +12864,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -12913,7 +12905,7 @@
         <v>0.81595511259153497</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -12954,7 +12946,7 @@
         <v>0.77299617086321304</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -12995,7 +12987,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -13036,7 +13028,7 @@
         <v>0.65835584489725196</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -13092,12 +13084,12 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -13138,7 +13130,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -13179,7 +13171,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -13220,7 +13212,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -13261,7 +13253,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -13302,7 +13294,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -13343,7 +13335,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -13384,7 +13376,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -13425,7 +13417,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -13466,7 +13458,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -13507,7 +13499,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -13548,7 +13540,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -13589,7 +13581,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -13630,7 +13622,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -13671,7 +13663,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -13712,7 +13704,7 @@
         <v>2.2831050228310501E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -13753,7 +13745,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -13794,7 +13786,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -13835,7 +13827,7 @@
         <v>0.77915338816094504</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -13876,7 +13868,7 @@
         <v>0.63024757853709501</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -13917,7 +13909,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -13958,7 +13950,7 @@
         <v>0.59834963673469899</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -13999,7 +13991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -14040,7 +14032,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -14081,7 +14073,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -14122,7 +14114,7 @@
         <v>0.77915338816094504</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -14163,7 +14155,7 @@
         <v>0.63024757853709501</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -14204,7 +14196,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -14245,7 +14237,7 @@
         <v>0.59834963673469899</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Industry CCS + high solar PV
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs_Trans.xlsx
@@ -1264,34 +1264,34 @@
     <t>S-LIG*, S-REF*, S-OEL*, S-PLIG*</t>
   </si>
   <si>
+    <t>S-LIG-PU_ELC_X0</t>
+  </si>
+  <si>
+    <t>S-LIG-CS_ELC_X0</t>
+  </si>
+  <si>
     <t>S-OEL-PU_ELC_X0</t>
   </si>
   <si>
     <t>S-OEL-CS_ELC_X0</t>
   </si>
   <si>
+    <t>S-PLIG-PU_X2</t>
+  </si>
+  <si>
+    <t>S-PLIG-PU_X1</t>
+  </si>
+  <si>
+    <t>S-PLIG-PU_X4</t>
+  </si>
+  <si>
+    <t>S-PLIG-PU_X3</t>
+  </si>
+  <si>
     <t>S-REF-PU_ELC_X0</t>
   </si>
   <si>
     <t>S-REF-CS_ELC_X0</t>
-  </si>
-  <si>
-    <t>S-LIG-PU_ELC_X0</t>
-  </si>
-  <si>
-    <t>S-LIG-CS_ELC_X0</t>
-  </si>
-  <si>
-    <t>S-PLIG-PU_X2</t>
-  </si>
-  <si>
-    <t>S-PLIG-PU_X1</t>
-  </si>
-  <si>
-    <t>S-PLIG-PU_X4</t>
-  </si>
-  <si>
-    <t>S-PLIG-PU_X3</t>
   </si>
   <si>
     <t>*Electric appliances</t>
@@ -1514,14 +1514,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.499550014734268"/>
+      <color theme="7" tint="-0.499529987573624"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.499550014734268"/>
+      <color theme="7" tint="-0.499529987573624"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1556,7 +1556,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0495599992573261"/>
+        <fgColor theme="0" tint="-0.0495399981737137"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1610,7 +1610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149570003151894"/>
+        <fgColor theme="0" tint="-0.149550005793571"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2258,7 +2258,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="4554" t="8869" r="7682" b="12861"/>
+        <a:srcRect l="4551" t="8866" r="7679" b="12858"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2385,7 +2385,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId5"/>
-        <a:srcRect l="1304" t="6500" r="3947" b="6272"/>
+        <a:srcRect l="1301" t="6497" r="3944" b="6269"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2428,7 +2428,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId6"/>
-        <a:srcRect l="3935" t="26135" r="3935" b="26133"/>
+        <a:srcRect l="3932" t="26132" r="3932" b="26130"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6234,7 +6234,7 @@
         <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -6275,7 +6275,7 @@
         <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -6316,7 +6316,7 @@
         <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -6357,7 +6357,7 @@
         <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -6398,7 +6398,7 @@
         <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -6439,7 +6439,7 @@
         <v>127</v>
       </c>
       <c r="C7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -6480,7 +6480,7 @@
         <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -6521,7 +6521,7 @@
         <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -6562,7 +6562,7 @@
         <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -6603,7 +6603,7 @@
         <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -6644,7 +6644,7 @@
         <v>255</v>
       </c>
       <c r="C12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -6685,7 +6685,7 @@
         <v>255</v>
       </c>
       <c r="C13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -6726,7 +6726,7 @@
         <v>255</v>
       </c>
       <c r="C14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -6767,7 +6767,7 @@
         <v>255</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>

</xml_diff>